<commit_message>
Mapa de conceito Imunizacao
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/Modelo lógicoI ImunizacaoIPS.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/Modelo lógicoI ImunizacaoIPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Imunizacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Imunizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB869D6-CC66-EA48-A20B-8FED2DF6B258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33614FD7-DA89-4248-9BCA-46E96C3F89D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="1960" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa semântico" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2827" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2827" uniqueCount="1407">
   <si>
     <t>Mapeamento semântico</t>
   </si>
@@ -4246,13 +4246,19 @@
   </si>
   <si>
     <t>0..1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/R4/valueset-immunization-status.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://hl7.org/fhir/uv/ips/ValueSet/vaccines-snomed-ct-ips-free-set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4403,6 +4409,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF4A86E8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4606,10 +4620,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4697,8 +4712,10 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4818,6 +4835,372 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="image3.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{119544F0-2592-800A-E00C-AB706ED94A27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3257564-3026-EDBB-17A2-BBDDDCE8D25A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B7F163-FA67-70DE-9CBC-840EA50BCB6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA7BC959-33F2-F0B0-FB8F-F84B2C00EF5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1029" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{314F2BA3-534D-0DC7-3E8D-3FD290FB0CA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BDFC747-820C-97F9-2DEE-D65B17244EAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7797800" y="1079500"/>
+          <a:ext cx="406400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5383,14 +5766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5483,8 +5866,8 @@
       <c r="F4" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="47" t="s">
-        <v>12</v>
+      <c r="G4" s="59" t="s">
+        <v>1405</v>
       </c>
       <c r="H4" s="48" t="s">
         <v>13</v>
@@ -5512,8 +5895,8 @@
       <c r="F5" s="51" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="47" t="s">
-        <v>16</v>
+      <c r="G5" s="59" t="s">
+        <v>1406</v>
       </c>
       <c r="H5" s="48" t="s">
         <v>17</v>
@@ -5858,7 +6241,7 @@
     <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="H4" location="'ConceptMapimmunization-status'!A1" display="ConceptMap/immunization-status" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G5" r:id="rId4" display="http://www.saude.gov." xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="H5" location="'ConceptMapvaccine-code'!A1" display="ConceptMap/immunization-vaccine-code" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="A10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="H10" location="'ConceptMapimmunization-report-o'!A1" display="ConceptMap/immunization-report-origin" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
@@ -5872,7 +6255,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Results Microorganisms carga HL7
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/Modelo lógicoI ImunizacaoIPS.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/Modelo lógicoI ImunizacaoIPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Imunizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8990AA5-33C4-604D-B932-618B24007866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D07C5F-E26E-5547-A4C4-9502D29DDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="1320" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa semântico" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="1417">
   <si>
     <t>Mapeamento semântico</t>
   </si>
@@ -4292,6 +4292,9 @@
   </si>
   <si>
     <t>Traduzir no valueSet</t>
+  </si>
+  <si>
+    <t>Só exemplo. Nãos erá utilizado no IPS</t>
   </si>
 </sst>
 </file>
@@ -5821,10 +5824,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5839,7 +5842,7 @@
     <col min="9" max="9" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="78.75" customHeight="1">
+    <row r="1" spans="1:16" ht="78.75" customHeight="1">
       <c r="A1" s="33"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -5852,7 +5855,7 @@
       <c r="H1" s="37"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="34.5" customHeight="1">
+    <row r="2" spans="1:16" ht="34.5" customHeight="1">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
@@ -5871,7 +5874,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="16">
+    <row r="3" spans="1:16" ht="16">
       <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16">
+    <row r="4" spans="1:16" ht="16">
       <c r="A4" s="60" t="s">
         <v>12</v>
       </c>
@@ -5933,7 +5936,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16">
+    <row r="5" spans="1:16" ht="16">
       <c r="A5" s="60" t="s">
         <v>16</v>
       </c>
@@ -5962,7 +5965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16">
+    <row r="6" spans="1:16" ht="16">
       <c r="A6" s="52" t="s">
         <v>18</v>
       </c>
@@ -5989,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16">
+    <row r="7" spans="1:16" ht="16">
       <c r="A7" s="52" t="s">
         <v>18</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16">
+    <row r="8" spans="1:16" ht="16">
       <c r="A8" s="52" t="s">
         <v>18</v>
       </c>
@@ -6043,7 +6046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16">
+    <row r="9" spans="1:16" ht="16">
       <c r="A9" s="52" t="s">
         <v>18</v>
       </c>
@@ -6070,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16">
+    <row r="10" spans="1:16" ht="16">
       <c r="A10" s="43" t="s">
         <v>23</v>
       </c>
@@ -6099,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16">
+    <row r="11" spans="1:16" ht="16">
       <c r="A11" s="52" t="s">
         <v>18</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16">
+    <row r="12" spans="1:16" ht="16">
       <c r="A12" s="52" t="s">
         <v>18</v>
       </c>
@@ -6153,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16">
+    <row r="13" spans="1:16" ht="16">
       <c r="A13" s="52" t="s">
         <v>18</v>
       </c>
@@ -6180,7 +6183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16">
+    <row r="14" spans="1:16" ht="16">
       <c r="A14" s="43" t="s">
         <v>30</v>
       </c>
@@ -6212,7 +6215,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16">
+    <row r="15" spans="1:16" ht="16">
       <c r="A15" s="43" t="s">
         <v>34</v>
       </c>
@@ -6243,8 +6246,11 @@
       <c r="J15" s="61" t="s">
         <v>1413</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="16">
+      <c r="P15" s="61" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16">
       <c r="A16" s="52" t="s">
         <v>18</v>
       </c>

</xml_diff>